<commit_message>
Update chart code and README
</commit_message>
<xml_diff>
--- a/student_marks.xlsx
+++ b/student_marks.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUBHRA\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -22,18 +27,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Math</t>
-  </si>
-  <si>
-    <t>Physics</t>
-  </si>
-  <si>
-    <t>Chemistry</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
     <t>S001</t>
   </si>
   <si>
@@ -272,13 +265,25 @@
   </si>
   <si>
     <t>Student_40</t>
+  </si>
+  <si>
+    <t>ADMS</t>
+  </si>
+  <si>
+    <t>AOS</t>
+  </si>
+  <si>
+    <t>A&amp;CD</t>
+  </si>
+  <si>
+    <t>C&amp;NS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +346,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -387,7 +400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,9 +432,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,6 +467,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -628,14 +643,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,24 +660,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>51</v>
@@ -675,12 +692,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -695,12 +712,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -715,12 +732,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>71</v>
@@ -732,21 +749,21 @@
         <v>33</v>
       </c>
       <c r="F5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>60</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>73</v>
@@ -755,12 +772,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -775,12 +792,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>82</v>
@@ -792,21 +809,21 @@
         <v>99</v>
       </c>
       <c r="F8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>86</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E9">
         <v>13</v>
@@ -815,12 +832,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>74</v>
@@ -835,12 +852,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C11">
         <v>74</v>
@@ -855,12 +872,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C12">
         <v>87</v>
@@ -875,12 +892,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C13">
         <v>99</v>
@@ -895,18 +912,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C14">
         <v>23</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E14">
         <v>77</v>
@@ -915,15 +932,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <v>88</v>
@@ -935,12 +952,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <v>21</v>
@@ -955,12 +972,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17">
         <v>52</v>
@@ -975,18 +992,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E18">
         <v>84</v>
@@ -995,32 +1012,32 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D19">
         <v>89</v>
       </c>
       <c r="E19">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F19">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20">
         <v>29</v>
@@ -1035,18 +1052,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>37</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E21">
         <v>52</v>
@@ -1055,15 +1072,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D22">
         <v>83</v>
@@ -1075,12 +1092,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C23">
         <v>63</v>
@@ -1095,12 +1112,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C24">
         <v>59</v>
@@ -1115,12 +1132,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C25">
         <v>20</v>
@@ -1135,12 +1152,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C26">
         <v>32</v>
@@ -1155,18 +1172,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C27">
         <v>75</v>
       </c>
       <c r="D27">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E27">
         <v>28</v>
@@ -1175,12 +1192,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C28">
         <v>57</v>
@@ -1195,12 +1212,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C29">
         <v>21</v>
@@ -1212,15 +1229,15 @@
         <v>44</v>
       </c>
       <c r="F29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C30">
         <v>88</v>
@@ -1232,18 +1249,18 @@
         <v>64</v>
       </c>
       <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="D31">
         <v>80</v>
@@ -1252,15 +1269,15 @@
         <v>88</v>
       </c>
       <c r="F31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C32">
         <v>90</v>
@@ -1275,12 +1292,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C33">
         <v>58</v>
@@ -1289,24 +1306,24 @@
         <v>49</v>
       </c>
       <c r="E33">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F33">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C34">
         <v>41</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E34">
         <v>87</v>
@@ -1315,52 +1332,52 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C35">
         <v>91</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F35">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C36">
         <v>59</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E36">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F36">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C37">
         <v>79</v>
@@ -1375,18 +1392,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38">
         <v>14</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E38">
         <v>62</v>
@@ -1395,12 +1412,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C39">
         <v>61</v>
@@ -1415,32 +1432,32 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C40">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D40">
         <v>92</v>
       </c>
       <c r="E40">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F40">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C41">
         <v>46</v>
@@ -1449,7 +1466,7 @@
         <v>62</v>
       </c>
       <c r="E41">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F41">
         <v>50</v>

</xml_diff>